<commit_message>
Update name of skill level
</commit_message>
<xml_diff>
--- a/data-raw/datalist_en.xlsx
+++ b/data-raw/datalist_en.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B884DAD-9888-4625-8419-219C11B20182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="1800" windowWidth="14400" windowHeight="8190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_information" sheetId="2" r:id="rId1"/>
@@ -857,23 +857,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="21.875" customWidth="1"/>
     <col min="2" max="2" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.7">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="12"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A3" s="12" t="s">
         <v>22</v>
       </c>
@@ -881,11 +881,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
@@ -904,9 +904,11 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:W161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="6.375" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
@@ -928,7 +930,7 @@
     <col min="19" max="23" width="8.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="213.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="217" thickBot="1" x14ac:dyDescent="0.8">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -999,151 +1001,151 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="23" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="104" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="105" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="106" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="107" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="108" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="109" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="110" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="111" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="112" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="145" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="146" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="147" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="148" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="149" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="150" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="151" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="152" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="153" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="154" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="155" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="156" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="157" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="158" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="159" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="160" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="161" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="145" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="146" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="147" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="148" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="149" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="150" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="151" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="152" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="153" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="154" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="155" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="156" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="157" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="158" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="159" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="160" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="161" customFormat="1" x14ac:dyDescent="0.65"/>
   </sheetData>
   <autoFilter ref="A1:W161" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W161">

</xml_diff>